<commit_message>
test it in windows, left with a problem of style
</commit_message>
<xml_diff>
--- a/demo/test.xlsx
+++ b/demo/test.xlsx
@@ -1,47 +1,111 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="9340"/>
+  </bookViews>
   <sheets>
-    <sheet name="SheetJS" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>sheetjs</t>
-  </si>
-  <si>
-    <t>foo</t>
-  </si>
-  <si>
-    <t>bar</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>baz</t>
-  </si>
-  <si>
-    <t>qux</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+  <si>
+    <t>Hi,{name}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>His name is {name} and {age} years old.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{average}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{students.name}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{students.age}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{name1}</t>
+  </si>
+  <si>
+    <t>{age1}</t>
+  </si>
+  <si>
+    <t>{name2}</t>
+  </si>
+  <si>
+    <t>{age2}</t>
+  </si>
+  <si>
+    <t>{name3}</t>
+  </si>
+  <si>
+    <t>{age3}</t>
+  </si>
+  <si>
+    <t>{name4}</t>
+  </si>
+  <si>
+    <t>{age4}</t>
+  </si>
+  <si>
+    <t>{name5}</t>
+  </si>
+  <si>
+    <t>{age5}</t>
+  </si>
+  <si>
+    <t>{now}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -65,20 +129,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -120,7 +204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -155,7 +239,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,16 +306,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -353,102 +441,133 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="SheetJS"/>
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C7:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="43" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="1"/>
+    <col min="7" max="7" width="12.54296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.08984375" style="4" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1">
+      <c r="H11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="b">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="G12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
-        <v>41689.604166666664</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="G13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="G14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="1">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="1">
         <v>5</v>
       </c>
+      <c r="G16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: use exceljs instead of xlsx
</commit_message>
<xml_diff>
--- a/demo/test.xlsx
+++ b/demo/test.xlsx
@@ -1,132 +1,483 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="20490" windowHeight="9340"/>
+    <workbookView windowWidth="28000" windowHeight="11000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
+  <si>
+    <t>His name is {name} and {age} years old.</t>
+  </si>
+  <si>
+    <t>{fields.name}</t>
+  </si>
   <si>
     <t>Hi,{name}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>His name is {name} and {age} years old.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{now}</t>
+  </si>
+  <si>
+    <t>{isBoy}</t>
+  </si>
+  <si>
+    <t>{isGirl}</t>
   </si>
   <si>
     <t>Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Age</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rich </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <charset val="134"/>
+      </rPr>
+      <t>text</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> {name}</t>
+    </r>
+  </si>
+  <si>
+    <t>{name1}</t>
+  </si>
+  <si>
+    <t>{age1}</t>
+  </si>
+  <si>
+    <t>{name2}</t>
+  </si>
+  <si>
+    <t>{age2}</t>
+  </si>
+  <si>
+    <t>{name3}</t>
+  </si>
+  <si>
+    <t>{age3}</t>
+  </si>
+  <si>
+    <t>{name4}</t>
+  </si>
+  <si>
+    <t>{age4}</t>
+  </si>
+  <si>
+    <t>{name5}</t>
+  </si>
+  <si>
+    <t>{age5}</t>
   </si>
   <si>
     <t>Average</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>{average}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Age</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>{students.name}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>{students.age}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{name1}</t>
-  </si>
-  <si>
-    <t>{age1}</t>
-  </si>
-  <si>
-    <t>{name2}</t>
-  </si>
-  <si>
-    <t>{age2}</t>
-  </si>
-  <si>
-    <t>{name3}</t>
-  </si>
-  <si>
-    <t>{age3}</t>
-  </si>
-  <si>
-    <t>{name4}</t>
-  </si>
-  <si>
-    <t>{age4}</t>
-  </si>
-  <si>
-    <t>{name5}</t>
-  </si>
-  <si>
-    <t>{age5}</t>
-  </si>
-  <si>
-    <t>{now}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{isBoy}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{isGirl}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0_ "/>
-    <numFmt numFmtId="178" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -134,11 +485,253 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -146,25 +739,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
+    <cellStyle name="Bad" xfId="22" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
+    <cellStyle name="Total" xfId="24" builtinId="25"/>
+    <cellStyle name="Output" xfId="25" builtinId="21"/>
+    <cellStyle name="Currency" xfId="26" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
+    <cellStyle name="Note" xfId="28" builtinId="10"/>
+    <cellStyle name="Input" xfId="29" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
+    <cellStyle name="Good" xfId="32" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="Title" xfId="38" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
+    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
+    <cellStyle name="Link" xfId="43" builtinId="8"/>
+    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
+    <cellStyle name="Comma" xfId="45" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -213,7 +851,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,7 +886,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -451,141 +1089,147 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="C7:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="3" max="3" width="43" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" style="1"/>
-    <col min="6" max="6" width="12.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.453125" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.7265625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.08984375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.09375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:9">
       <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:3">
       <c r="C8" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="5" t="s">
-        <v>19</v>
+    <row r="9" spans="3:3">
+      <c r="C9" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:3">
       <c r="C10" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:7">
       <c r="C11" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:7">
+      <c r="C12" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:7">
       <c r="E13" s="1">
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:7">
       <c r="E14" s="1">
         <v>3</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:7">
       <c r="E15" s="1">
         <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:7">
       <c r="E16" s="1">
         <v>5</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:7">
       <c r="E17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:10">
       <c r="I21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="J21" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:10">
       <c r="I22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>8</v>
+        <v>21</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>